<commit_message>
Finished migration of S25 stats, added some details to some templates, corrected leaders template
</commit_message>
<xml_diff>
--- a/D1_Schedule_Fall2025.xlsx
+++ b/D1_Schedule_Fall2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sbclaude\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7E9690-9D25-40AF-B6FC-94FEB48F5076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858C49F3-43C6-4477-8F3E-F5759C79FC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="224">
   <si>
     <t>Villages D1 Softball - Fall 2025</t>
   </si>
@@ -49,168 +49,36 @@
     <t>Friday, September 05</t>
   </si>
   <si>
-    <t>9:00 Xtreme at The Sandlot on 1</t>
-  </si>
-  <si>
-    <t>9:00 Shorebirds at Bad News Bears on 2</t>
-  </si>
-  <si>
-    <t>10:30 Buckeyes at Clippers on 1</t>
-  </si>
-  <si>
-    <t>10:30 Stars at Warhawks on 2</t>
-  </si>
-  <si>
     <t>Wednesday, September 10</t>
   </si>
   <si>
     <t>Friday, September 12</t>
   </si>
   <si>
-    <t>9:00 Raptors at Norsemen on 1</t>
-  </si>
-  <si>
-    <t>9:00 Lightning Strikes at Warhawks on 1</t>
-  </si>
-  <si>
-    <t>9:00 Bad News Bears at Buckeyes on 2</t>
-  </si>
-  <si>
-    <t>9:00 Buckeyes at Xtreme on 2</t>
-  </si>
-  <si>
-    <t>10:30 Stars at Lightning Strikes on 1</t>
-  </si>
-  <si>
-    <t>10:30 Shorebirds at The Sandlot on 1</t>
-  </si>
-  <si>
-    <t>10:30 Clippers at Rebels on 2</t>
-  </si>
-  <si>
-    <t>10:30 Norsemen at Clippers on 2</t>
-  </si>
-  <si>
     <t>Wednesday, September 17</t>
   </si>
   <si>
     <t>Friday, September 19</t>
   </si>
   <si>
-    <t>9:00 Clippers at Stars on 1</t>
-  </si>
-  <si>
-    <t>9:00 Rebels at Shorebirds on 1</t>
-  </si>
-  <si>
-    <t>9:00 The Sandlot at Lightning Strikes on 2</t>
-  </si>
-  <si>
-    <t>9:00 Norsemen at Xtreme on 2</t>
-  </si>
-  <si>
-    <t>10:30 Xtreme at Rebels on 1</t>
-  </si>
-  <si>
-    <t>10:30 Stars at Bad News Bears on 1</t>
-  </si>
-  <si>
-    <t>10:30 Raptors at Warhawks on 2</t>
-  </si>
-  <si>
-    <t>10:30 Lightning Strikes at Raptors on 2</t>
-  </si>
-  <si>
     <t>Wednesday, September 24</t>
   </si>
   <si>
     <t>Friday, September 26</t>
   </si>
   <si>
-    <t>9:00 Rebels at Buckeyes on 1</t>
-  </si>
-  <si>
-    <t>9:00 Bad News Bears at Lightning Strikes on 1</t>
-  </si>
-  <si>
-    <t>9:00 The Sandlot at Raptors on 2</t>
-  </si>
-  <si>
-    <t>9:00 Rebels at The Sandlot on 2</t>
-  </si>
-  <si>
-    <t>10:30 Norsemen at Shorebirds on 1</t>
-  </si>
-  <si>
-    <t>10:30 Norsemen at Buckeyes on 1</t>
-  </si>
-  <si>
-    <t>10:30 Warhawks at Bad News Bears on 2</t>
-  </si>
-  <si>
-    <t>10:30 Warhawks at Xtreme on 2</t>
-  </si>
-  <si>
     <t>Wednesday, October 01</t>
   </si>
   <si>
     <t>Friday, October 03</t>
   </si>
   <si>
-    <t>9:00 Bad News Bears at Raptors on 1</t>
-  </si>
-  <si>
-    <t>9:00 Xtreme at Raptors on 1</t>
-  </si>
-  <si>
-    <t>9:00 Rebels at Norsemen on 2</t>
-  </si>
-  <si>
-    <t>9:00 Bad News Bears at Clippers on 2</t>
-  </si>
-  <si>
-    <t>10:30 Clippers at The Sandlot on 1</t>
-  </si>
-  <si>
-    <t>10:30 Warhawks at Buckeyes on 1</t>
-  </si>
-  <si>
-    <t>10:30 Buckeyes at Stars on 2</t>
-  </si>
-  <si>
-    <t>10:30 Shorebirds at Lightning Strikes on 2</t>
-  </si>
-  <si>
     <t>Wednesday, October 08</t>
   </si>
   <si>
     <t>Friday, October 10</t>
   </si>
   <si>
-    <t>9:00 Xtreme at Clippers on 1</t>
-  </si>
-  <si>
-    <t>9:00 Stars at The Sandlot on 1</t>
-  </si>
-  <si>
-    <t>9:00 Stars at Norsemen on 2</t>
-  </si>
-  <si>
-    <t>9:00 Warhawks at Norsemen on 2</t>
-  </si>
-  <si>
-    <t>10:30 Warhawks at Rebels on 1</t>
-  </si>
-  <si>
-    <t>10:30 Lightning Strikes at Rebels on 1</t>
-  </si>
-  <si>
-    <t>10:30 Shorebirds at Raptors on 2</t>
-  </si>
-  <si>
-    <t>10:30 Shorebirds at Clippers on 2</t>
-  </si>
-  <si>
     <t>Schedule - Second Half</t>
   </si>
   <si>
@@ -220,168 +88,36 @@
     <t>Friday, October 17</t>
   </si>
   <si>
-    <t>9:00 Warhawks at Stars on 1</t>
-  </si>
-  <si>
-    <t>9:00 Raptors at Rebels on 2</t>
-  </si>
-  <si>
-    <t>10:30 Bad News Bears at Shorebirds on 1</t>
-  </si>
-  <si>
-    <t>10:30 The Sandlot at Xtreme on 2</t>
-  </si>
-  <si>
     <t>Wednesday, October 22</t>
   </si>
   <si>
     <t>Friday, October 24</t>
   </si>
   <si>
-    <t>9:00 Xtreme at Shorebirds on 1</t>
-  </si>
-  <si>
-    <t>9:00 Clippers at Norsemen on 1</t>
-  </si>
-  <si>
-    <t>9:00 Buckeyes at Bad News Bears on 2</t>
-  </si>
-  <si>
-    <t>9:00 The Sandlot at Shorebirds on 2</t>
-  </si>
-  <si>
-    <t>10:30 Norsemen at Raptors on 1</t>
-  </si>
-  <si>
-    <t>10:30 Bad News Bears at Rebels on 1</t>
-  </si>
-  <si>
-    <t>10:30 Lightning Strikes at Stars on 2</t>
-  </si>
-  <si>
-    <t>10:30 Xtreme at Buckeyes on 2</t>
-  </si>
-  <si>
     <t>Wednesday, October 29</t>
   </si>
   <si>
     <t>Friday, October 31</t>
   </si>
   <si>
-    <t>9:00 Lightning Strikes at The Sandlot on 1</t>
-  </si>
-  <si>
-    <t>9:00 Raptors at Lightning Strikes on 1</t>
-  </si>
-  <si>
-    <t>9:00 Warhawks at Raptors on 2</t>
-  </si>
-  <si>
-    <t>9:00 Bad News Bears at Stars on 2</t>
-  </si>
-  <si>
-    <t>10:30 Shorebirds at Buckeyes on 1</t>
-  </si>
-  <si>
-    <t>10:30 Warhawks at Clippers on 1</t>
-  </si>
-  <si>
-    <t>10:30 Stars at Clippers on 2</t>
-  </si>
-  <si>
-    <t>10:30 Shorebirds at Rebels on 2</t>
-  </si>
-  <si>
     <t>Wednesday, November 05</t>
   </si>
   <si>
     <t>Friday, November 07</t>
   </si>
   <si>
-    <t>9:00 Bad News Bears at Warhawks on 1</t>
-  </si>
-  <si>
-    <t>9:00 Buckeyes at Norsemen on 1</t>
-  </si>
-  <si>
-    <t>9:00 Stars at Xtreme on 2</t>
-  </si>
-  <si>
-    <t>9:00 Clippers at Raptors on 2</t>
-  </si>
-  <si>
-    <t>10:30 Raptors at The Sandlot on 1</t>
-  </si>
-  <si>
-    <t>10:30 Xtreme at Warhawks on 1</t>
-  </si>
-  <si>
-    <t>10:30 Buckeyes at Rebels on 2</t>
-  </si>
-  <si>
-    <t>10:30 Lightning Strikes at Bad News Bears on 2</t>
-  </si>
-  <si>
     <t>Wednesday, November 12</t>
   </si>
   <si>
     <t>Friday, November 14</t>
   </si>
   <si>
-    <t>9:00 Stars at Buckeyes on 1</t>
-  </si>
-  <si>
-    <t>9:00 Clippers at Bad News Bears on 1</t>
-  </si>
-  <si>
-    <t>9:00 Norsemen at Rebels on 2</t>
-  </si>
-  <si>
-    <t>9:00 Lightning Strikes at Shorebirds on 2</t>
-  </si>
-  <si>
-    <t>10:30 Lightning Strikes at Xtreme on 1</t>
-  </si>
-  <si>
-    <t>10:30 Norsemen at The Sandlot on 1</t>
-  </si>
-  <si>
-    <t>10:30 The Sandlot at Clippers on 2</t>
-  </si>
-  <si>
-    <t>10:30 Buckeyes at Warhawks on 2</t>
-  </si>
-  <si>
     <t>Wednesday, November 19</t>
   </si>
   <si>
     <t>Friday, November 21</t>
   </si>
   <si>
-    <t>9:00 Norsemen at Stars on 1</t>
-  </si>
-  <si>
-    <t>9:00 Clippers at Shorebirds on 1</t>
-  </si>
-  <si>
-    <t>9:00 The Sandlot at Bad News Bears on 2</t>
-  </si>
-  <si>
-    <t>9:00 Norsemen at Warhawks on 2</t>
-  </si>
-  <si>
-    <t>10:30 Rebels at Warhawks on 1</t>
-  </si>
-  <si>
-    <t>10:30 The Sandlot at Stars on 1</t>
-  </si>
-  <si>
-    <t>10:30 Raptors at Shorebirds on 2</t>
-  </si>
-  <si>
-    <t>10:30 Bad News Bears at Xtreme on 2</t>
-  </si>
-  <si>
     <t>Wednesday, November 26</t>
   </si>
   <si>
@@ -451,18 +187,12 @@
     <t>Fri</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Xtreme</t>
   </si>
   <si>
     <t>The Sandlot</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Shorebirds</t>
   </si>
   <si>
@@ -713,6 +443,270 @@
   </si>
   <si>
     <t>10:30 Raptors at Buckeyes on 4</t>
+  </si>
+  <si>
+    <t>9:00 Shorebirds at Bad News Bears on 3</t>
+  </si>
+  <si>
+    <t>10:30 Stars at Warhawks on 3</t>
+  </si>
+  <si>
+    <t>9:00 Bad News Bears at Buckeyes on 3</t>
+  </si>
+  <si>
+    <t>9:00 Buckeyes at Xtreme on 3</t>
+  </si>
+  <si>
+    <t>10:30 Clippers at Rebels on 3</t>
+  </si>
+  <si>
+    <t>10:30 Norsemen at Clippers on 3</t>
+  </si>
+  <si>
+    <t>9:00 The Sandlot at Lightning Strikes on 3</t>
+  </si>
+  <si>
+    <t>9:00 Norsemen at Xtreme on 3</t>
+  </si>
+  <si>
+    <t>10:30 Raptors at Warhawks on 3</t>
+  </si>
+  <si>
+    <t>10:30 Lightning Strikes at Raptors on 3</t>
+  </si>
+  <si>
+    <t>9:00 The Sandlot at Raptors on 3</t>
+  </si>
+  <si>
+    <t>9:00 Rebels at The Sandlot on 3</t>
+  </si>
+  <si>
+    <t>10:30 Warhawks at Bad News Bears on 3</t>
+  </si>
+  <si>
+    <t>10:30 Warhawks at Xtreme on 3</t>
+  </si>
+  <si>
+    <t>9:00 Rebels at Norsemen on 3</t>
+  </si>
+  <si>
+    <t>9:00 Bad News Bears at Clippers on 3</t>
+  </si>
+  <si>
+    <t>10:30 Buckeyes at Stars on 3</t>
+  </si>
+  <si>
+    <t>10:30 Shorebirds at Lightning Strikes on 3</t>
+  </si>
+  <si>
+    <t>9:00 Stars at Norsemen on 3</t>
+  </si>
+  <si>
+    <t>9:00 Warhawks at Norsemen on 3</t>
+  </si>
+  <si>
+    <t>10:30 Shorebirds at Raptors on 3</t>
+  </si>
+  <si>
+    <t>10:30 Shorebirds at Clippers on 3</t>
+  </si>
+  <si>
+    <t>9:00 Raptors at Rebels on 3</t>
+  </si>
+  <si>
+    <t>10:30 The Sandlot at Xtreme on 3</t>
+  </si>
+  <si>
+    <t>9:00 Buckeyes at Bad News Bears on 3</t>
+  </si>
+  <si>
+    <t>9:00 The Sandlot at Shorebirds on 3</t>
+  </si>
+  <si>
+    <t>10:30 Lightning Strikes at Stars on 3</t>
+  </si>
+  <si>
+    <t>10:30 Xtreme at Buckeyes on 3</t>
+  </si>
+  <si>
+    <t>9:00 Warhawks at Raptors on 3</t>
+  </si>
+  <si>
+    <t>9:00 Bad News Bears at Stars on 3</t>
+  </si>
+  <si>
+    <t>10:30 Stars at Clippers on 3</t>
+  </si>
+  <si>
+    <t>10:30 Shorebirds at Rebels on 3</t>
+  </si>
+  <si>
+    <t>9:00 Stars at Xtreme on 3</t>
+  </si>
+  <si>
+    <t>9:00 Clippers at Raptors on 3</t>
+  </si>
+  <si>
+    <t>10:30 Buckeyes at Rebels on 3</t>
+  </si>
+  <si>
+    <t>10:30 Lightning Strikes at Bad News Bears on 3</t>
+  </si>
+  <si>
+    <t>9:00 Norsemen at Rebels on 3</t>
+  </si>
+  <si>
+    <t>9:00 Lightning Strikes at Shorebirds on 3</t>
+  </si>
+  <si>
+    <t>10:30 The Sandlot at Clippers on 3</t>
+  </si>
+  <si>
+    <t>10:30 Buckeyes at Warhawks on 3</t>
+  </si>
+  <si>
+    <t>9:00 The Sandlot at Bad News Bears on 3</t>
+  </si>
+  <si>
+    <t>9:00 Norsemen at Warhawks on 3</t>
+  </si>
+  <si>
+    <t>10:30 Raptors at Shorebirds on 3</t>
+  </si>
+  <si>
+    <t>10:30 Bad News Bears at Xtreme on 3</t>
+  </si>
+  <si>
+    <t>9:00 Warhawks at Stars on 2</t>
+  </si>
+  <si>
+    <t>10:30 Bad News Bears at Shorebirds on 2</t>
+  </si>
+  <si>
+    <t>9:00 Xtreme at Shorebirds on 2</t>
+  </si>
+  <si>
+    <t>9:00 Clippers at Norsemen on 2</t>
+  </si>
+  <si>
+    <t>10:30 Norsemen at Raptors on 2</t>
+  </si>
+  <si>
+    <t>10:30 Bad News Bears at Rebels on 2</t>
+  </si>
+  <si>
+    <t>9:00 Lightning Strikes at The Sandlot on 2</t>
+  </si>
+  <si>
+    <t>9:00 Raptors at Lightning Strikes on 2</t>
+  </si>
+  <si>
+    <t>10:30 Shorebirds at Buckeyes on 2</t>
+  </si>
+  <si>
+    <t>10:30 Warhawks at Clippers on 2</t>
+  </si>
+  <si>
+    <t>9:00 Bad News Bears at Warhawks on 2</t>
+  </si>
+  <si>
+    <t>9:00 Buckeyes at Norsemen on 2</t>
+  </si>
+  <si>
+    <t>10:30 Raptors at The Sandlot on 2</t>
+  </si>
+  <si>
+    <t>10:30 Xtreme at Warhawks on 2</t>
+  </si>
+  <si>
+    <t>9:00 Stars at Buckeyes on 2</t>
+  </si>
+  <si>
+    <t>9:00 Clippers at Bad News Bears on 2</t>
+  </si>
+  <si>
+    <t>10:30 Lightning Strikes at Xtreme on 2</t>
+  </si>
+  <si>
+    <t>10:30 Norsemen at The Sandlot on 2</t>
+  </si>
+  <si>
+    <t>9:00 Norsemen at Stars on 2</t>
+  </si>
+  <si>
+    <t>9:00 Clippers at Shorebirds on 2</t>
+  </si>
+  <si>
+    <t>10:30 Rebels at Warhawks on 2</t>
+  </si>
+  <si>
+    <t>10:30 The Sandlot at Stars on 2</t>
+  </si>
+  <si>
+    <t>9:00 Xtreme at The Sandlot on 2</t>
+  </si>
+  <si>
+    <t>10:30 Buckeyes at Clippers on 2</t>
+  </si>
+  <si>
+    <t>9:00 Raptors at Norsemen on 2</t>
+  </si>
+  <si>
+    <t>9:00 Lightning Strikes at Warhawks on 2</t>
+  </si>
+  <si>
+    <t>10:30 Stars at Lightning Strikes on 2</t>
+  </si>
+  <si>
+    <t>10:30 Shorebirds at The Sandlot on 2</t>
+  </si>
+  <si>
+    <t>9:00 Clippers at Stars on 2</t>
+  </si>
+  <si>
+    <t>9:00 Rebels at Shorebirds on 2</t>
+  </si>
+  <si>
+    <t>10:30 Xtreme at Rebels on 2</t>
+  </si>
+  <si>
+    <t>10:30 Stars at Bad News Bears on 2</t>
+  </si>
+  <si>
+    <t>9:00 Rebels at Buckeyes on 2</t>
+  </si>
+  <si>
+    <t>9:00 Bad News Bears at Lightning Strikes on 2</t>
+  </si>
+  <si>
+    <t>10:30 Norsemen at Shorebirds on 2</t>
+  </si>
+  <si>
+    <t>10:30 Norsemen at Buckeyes on 2</t>
+  </si>
+  <si>
+    <t>9:00 Bad News Bears at Raptors on 2</t>
+  </si>
+  <si>
+    <t>9:00 Xtreme at Raptors on 2</t>
+  </si>
+  <si>
+    <t>10:30 Clippers at The Sandlot on 2</t>
+  </si>
+  <si>
+    <t>10:30 Warhawks at Buckeyes on 2</t>
+  </si>
+  <si>
+    <t>9:00 Xtreme at Clippers on 2</t>
+  </si>
+  <si>
+    <t>9:00 Stars at The Sandlot on 2</t>
+  </si>
+  <si>
+    <t>10:30 Warhawks at Rebels on 2</t>
+  </si>
+  <si>
+    <t>10:30 Lightning Strikes at Rebels on 2</t>
   </si>
 </sst>
 </file>
@@ -1373,8 +1367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:F55"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView showGridLines="0" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1432,7 +1426,7 @@
       <c r="B7" s="4"/>
       <c r="C7" s="20"/>
       <c r="E7" s="11" t="s">
-        <v>4</v>
+        <v>202</v>
       </c>
       <c r="F7" s="5"/>
     </row>
@@ -1440,17 +1434,17 @@
       <c r="B8" s="4"/>
       <c r="C8" s="7"/>
       <c r="E8" s="11" t="s">
-        <v>5</v>
+        <v>136</v>
       </c>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
       <c r="C9" s="23" t="s">
-        <v>125</v>
+        <v>37</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>182</v>
+        <v>92</v>
       </c>
       <c r="F9" s="5"/>
     </row>
@@ -1458,7 +1452,7 @@
       <c r="B10" s="4"/>
       <c r="C10" s="7"/>
       <c r="E10" s="11" t="s">
-        <v>6</v>
+        <v>203</v>
       </c>
       <c r="F10" s="5"/>
     </row>
@@ -1466,7 +1460,7 @@
       <c r="B11" s="4"/>
       <c r="C11" s="7"/>
       <c r="E11" s="11" t="s">
-        <v>7</v>
+        <v>137</v>
       </c>
       <c r="F11" s="5"/>
     </row>
@@ -1474,7 +1468,7 @@
       <c r="B12" s="4"/>
       <c r="C12" s="7"/>
       <c r="E12" s="11" t="s">
-        <v>183</v>
+        <v>93</v>
       </c>
       <c r="F12" s="5"/>
     </row>
@@ -1487,70 +1481,70 @@
     <row r="14" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
       <c r="C14" s="8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
       <c r="C15" s="12" t="s">
-        <v>10</v>
+        <v>204</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>11</v>
+        <v>205</v>
       </c>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="C16" s="12" t="s">
-        <v>12</v>
+        <v>138</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>13</v>
+        <v>139</v>
       </c>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="C17" s="12" t="s">
-        <v>184</v>
+        <v>94</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>185</v>
+        <v>95</v>
       </c>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="C18" s="12" t="s">
-        <v>14</v>
+        <v>206</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>15</v>
+        <v>207</v>
       </c>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="C19" s="12" t="s">
-        <v>16</v>
+        <v>140</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>17</v>
+        <v>141</v>
       </c>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
       <c r="C20" s="12" t="s">
-        <v>186</v>
+        <v>96</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>187</v>
+        <v>97</v>
       </c>
       <c r="F20" s="5"/>
     </row>
@@ -1563,70 +1557,70 @@
     <row r="22" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="8" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
       <c r="C23" s="12" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>21</v>
+        <v>209</v>
       </c>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
       <c r="C24" s="12" t="s">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>23</v>
+        <v>143</v>
       </c>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
       <c r="C25" s="12" t="s">
-        <v>188</v>
+        <v>98</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>189</v>
+        <v>99</v>
       </c>
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="C26" s="12" t="s">
-        <v>24</v>
+        <v>210</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>25</v>
+        <v>211</v>
       </c>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="C27" s="12" t="s">
-        <v>26</v>
+        <v>144</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>27</v>
+        <v>145</v>
       </c>
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
       <c r="C28" s="12" t="s">
-        <v>190</v>
+        <v>100</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>191</v>
+        <v>101</v>
       </c>
       <c r="F28" s="5"/>
     </row>
@@ -1639,70 +1633,70 @@
     <row r="30" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="C30" s="8" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
       <c r="C31" s="12" t="s">
-        <v>30</v>
+        <v>212</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>31</v>
+        <v>213</v>
       </c>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
       <c r="C32" s="12" t="s">
-        <v>32</v>
+        <v>146</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>33</v>
+        <v>147</v>
       </c>
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
       <c r="C33" s="12" t="s">
-        <v>192</v>
+        <v>102</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>193</v>
+        <v>103</v>
       </c>
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
       <c r="C34" s="12" t="s">
-        <v>34</v>
+        <v>214</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>35</v>
+        <v>215</v>
       </c>
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
       <c r="C35" s="12" t="s">
-        <v>36</v>
+        <v>148</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>37</v>
+        <v>149</v>
       </c>
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
       <c r="C36" s="12" t="s">
-        <v>194</v>
+        <v>104</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>195</v>
+        <v>105</v>
       </c>
       <c r="F36" s="5"/>
     </row>
@@ -1715,70 +1709,70 @@
     <row r="38" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
       <c r="C38" s="8" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="F38" s="5"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
       <c r="C39" s="12" t="s">
-        <v>40</v>
+        <v>216</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>41</v>
+        <v>217</v>
       </c>
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
       <c r="C40" s="12" t="s">
-        <v>42</v>
+        <v>150</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>43</v>
+        <v>151</v>
       </c>
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
       <c r="C41" s="12" t="s">
-        <v>196</v>
+        <v>106</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>197</v>
+        <v>107</v>
       </c>
       <c r="F41" s="5"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="4"/>
       <c r="C42" s="12" t="s">
-        <v>44</v>
+        <v>218</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>45</v>
+        <v>219</v>
       </c>
       <c r="F42" s="5"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
       <c r="C43" s="12" t="s">
-        <v>46</v>
+        <v>152</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>47</v>
+        <v>153</v>
       </c>
       <c r="F43" s="5"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
       <c r="C44" s="12" t="s">
-        <v>198</v>
+        <v>108</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>199</v>
+        <v>109</v>
       </c>
       <c r="F44" s="5"/>
     </row>
@@ -1791,70 +1785,70 @@
     <row r="46" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="4"/>
       <c r="C46" s="8" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="F46" s="5"/>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
       <c r="C47" s="12" t="s">
-        <v>50</v>
+        <v>220</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>51</v>
+        <v>221</v>
       </c>
       <c r="F47" s="5"/>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" s="4"/>
       <c r="C48" s="12" t="s">
-        <v>52</v>
+        <v>154</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>53</v>
+        <v>155</v>
       </c>
       <c r="F48" s="5"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="4"/>
       <c r="C49" s="12" t="s">
-        <v>200</v>
+        <v>110</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>201</v>
+        <v>111</v>
       </c>
       <c r="F49" s="5"/>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="4"/>
       <c r="C50" s="12" t="s">
-        <v>54</v>
+        <v>222</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>55</v>
+        <v>223</v>
       </c>
       <c r="F50" s="5"/>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" s="4"/>
       <c r="C51" s="12" t="s">
-        <v>56</v>
+        <v>156</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>57</v>
+        <v>157</v>
       </c>
       <c r="F51" s="5"/>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="4"/>
       <c r="C52" s="12" t="s">
-        <v>202</v>
+        <v>112</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>203</v>
+        <v>113</v>
       </c>
       <c r="F52" s="5"/>
     </row>
@@ -1891,8 +1885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:F64"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView showGridLines="0" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1924,7 +1918,7 @@
     <row r="4" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
       <c r="C4" s="29" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="D4" s="30"/>
       <c r="E4" s="31"/>
@@ -1939,17 +1933,17 @@
     <row r="6" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="8" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="12" t="s">
-        <v>61</v>
+        <v>180</v>
       </c>
       <c r="E7" s="21"/>
       <c r="F7" s="5"/>
@@ -1957,7 +1951,7 @@
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="C8" s="12" t="s">
-        <v>62</v>
+        <v>158</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="5"/>
@@ -1965,27 +1959,27 @@
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
       <c r="C9" s="12" t="s">
-        <v>204</v>
+        <v>114</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>126</v>
+        <v>38</v>
       </c>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
       <c r="C10" s="12" t="s">
-        <v>63</v>
+        <v>181</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>127</v>
+        <v>39</v>
       </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
       <c r="C11" s="12" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="5"/>
@@ -1993,7 +1987,7 @@
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="12" t="s">
-        <v>205</v>
+        <v>115</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="5"/>
@@ -2007,70 +2001,70 @@
     <row r="14" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
       <c r="C14" s="8" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
       <c r="C15" s="12" t="s">
-        <v>67</v>
+        <v>182</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>68</v>
+        <v>183</v>
       </c>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="C16" s="12" t="s">
-        <v>69</v>
+        <v>160</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>70</v>
+        <v>161</v>
       </c>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="C17" s="12" t="s">
-        <v>206</v>
+        <v>116</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>207</v>
+        <v>117</v>
       </c>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="C18" s="12" t="s">
-        <v>71</v>
+        <v>184</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>72</v>
+        <v>185</v>
       </c>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="C19" s="12" t="s">
-        <v>73</v>
+        <v>162</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>74</v>
+        <v>163</v>
       </c>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
       <c r="C20" s="12" t="s">
-        <v>208</v>
+        <v>118</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>209</v>
+        <v>119</v>
       </c>
       <c r="F20" s="5"/>
     </row>
@@ -2083,70 +2077,70 @@
     <row r="22" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="8" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
       <c r="C23" s="12" t="s">
-        <v>77</v>
+        <v>186</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>78</v>
+        <v>187</v>
       </c>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
       <c r="C24" s="12" t="s">
-        <v>79</v>
+        <v>164</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>80</v>
+        <v>165</v>
       </c>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
       <c r="C25" s="12" t="s">
-        <v>210</v>
+        <v>120</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>211</v>
+        <v>121</v>
       </c>
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="C26" s="12" t="s">
-        <v>81</v>
+        <v>188</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>82</v>
+        <v>189</v>
       </c>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="C27" s="12" t="s">
-        <v>83</v>
+        <v>166</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>84</v>
+        <v>167</v>
       </c>
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
       <c r="C28" s="12" t="s">
-        <v>212</v>
+        <v>122</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>213</v>
+        <v>123</v>
       </c>
       <c r="F28" s="5"/>
     </row>
@@ -2159,70 +2153,70 @@
     <row r="30" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="C30" s="8" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
       <c r="C31" s="12" t="s">
-        <v>87</v>
+        <v>190</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>88</v>
+        <v>191</v>
       </c>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
       <c r="C32" s="12" t="s">
-        <v>89</v>
+        <v>168</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>90</v>
+        <v>169</v>
       </c>
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
       <c r="C33" s="12" t="s">
-        <v>214</v>
+        <v>124</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>215</v>
+        <v>125</v>
       </c>
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
       <c r="C34" s="12" t="s">
-        <v>91</v>
+        <v>192</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>92</v>
+        <v>193</v>
       </c>
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
       <c r="C35" s="12" t="s">
-        <v>93</v>
+        <v>170</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>94</v>
+        <v>171</v>
       </c>
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
       <c r="C36" s="12" t="s">
-        <v>216</v>
+        <v>126</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>217</v>
+        <v>127</v>
       </c>
       <c r="F36" s="5"/>
     </row>
@@ -2235,70 +2229,70 @@
     <row r="38" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
       <c r="C38" s="8" t="s">
-        <v>95</v>
+        <v>23</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="F38" s="5"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
       <c r="C39" s="12" t="s">
-        <v>97</v>
+        <v>194</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>98</v>
+        <v>195</v>
       </c>
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
       <c r="C40" s="12" t="s">
-        <v>99</v>
+        <v>172</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>100</v>
+        <v>173</v>
       </c>
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
       <c r="C41" s="12" t="s">
-        <v>218</v>
+        <v>128</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>219</v>
+        <v>129</v>
       </c>
       <c r="F41" s="5"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="4"/>
       <c r="C42" s="12" t="s">
-        <v>101</v>
+        <v>196</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>102</v>
+        <v>197</v>
       </c>
       <c r="F42" s="5"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
       <c r="C43" s="12" t="s">
-        <v>103</v>
+        <v>174</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>104</v>
+        <v>175</v>
       </c>
       <c r="F43" s="5"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
       <c r="C44" s="12" t="s">
-        <v>220</v>
+        <v>130</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>221</v>
+        <v>131</v>
       </c>
       <c r="F44" s="5"/>
     </row>
@@ -2311,70 +2305,70 @@
     <row r="46" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="4"/>
       <c r="C46" s="8" t="s">
-        <v>105</v>
+        <v>25</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>106</v>
+        <v>26</v>
       </c>
       <c r="F46" s="5"/>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
       <c r="C47" s="12" t="s">
-        <v>107</v>
+        <v>198</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>108</v>
+        <v>199</v>
       </c>
       <c r="F47" s="5"/>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" s="4"/>
       <c r="C48" s="12" t="s">
-        <v>109</v>
+        <v>176</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>110</v>
+        <v>177</v>
       </c>
       <c r="F48" s="5"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="4"/>
       <c r="C49" s="12" t="s">
-        <v>222</v>
+        <v>132</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>223</v>
+        <v>133</v>
       </c>
       <c r="F49" s="5"/>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="4"/>
       <c r="C50" s="12" t="s">
-        <v>111</v>
+        <v>200</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>112</v>
+        <v>201</v>
       </c>
       <c r="F50" s="5"/>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" s="4"/>
       <c r="C51" s="12" t="s">
-        <v>113</v>
+        <v>178</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>114</v>
+        <v>179</v>
       </c>
       <c r="F51" s="5"/>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="4"/>
       <c r="C52" s="12" t="s">
-        <v>224</v>
+        <v>134</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>225</v>
+        <v>135</v>
       </c>
       <c r="F52" s="5"/>
     </row>
@@ -2387,20 +2381,20 @@
     <row r="54" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B54" s="4"/>
       <c r="C54" s="8" t="s">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>116</v>
+        <v>28</v>
       </c>
       <c r="F54" s="5"/>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="4"/>
       <c r="C55" s="10" t="s">
-        <v>117</v>
+        <v>29</v>
       </c>
       <c r="E55" s="19" t="s">
-        <v>118</v>
+        <v>30</v>
       </c>
       <c r="F55" s="5"/>
     </row>
@@ -2413,20 +2407,20 @@
     <row r="57" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="4"/>
       <c r="C57" s="8" t="s">
-        <v>119</v>
+        <v>31</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>120</v>
+        <v>32</v>
       </c>
       <c r="F57" s="5"/>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="4"/>
       <c r="C58" s="10" t="s">
-        <v>121</v>
+        <v>33</v>
       </c>
       <c r="E58" s="19" t="s">
-        <v>121</v>
+        <v>33</v>
       </c>
       <c r="F58" s="5"/>
     </row>
@@ -2439,20 +2433,20 @@
     <row r="60" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="4"/>
       <c r="C60" s="8" t="s">
-        <v>122</v>
+        <v>34</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>123</v>
+        <v>35</v>
       </c>
       <c r="F60" s="5"/>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="4"/>
       <c r="C61" s="10" t="s">
-        <v>124</v>
+        <v>36</v>
       </c>
       <c r="E61" s="19" t="s">
-        <v>124</v>
+        <v>36</v>
       </c>
       <c r="F61" s="5"/>
     </row>
@@ -2490,7 +2484,7 @@
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2514,7 +2508,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="37" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -2537,7 +2531,7 @@
     </row>
     <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>129</v>
+        <v>41</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
@@ -2562,7 +2556,7 @@
       <c r="A3" s="24"/>
       <c r="B3" s="24"/>
       <c r="C3" s="39" t="s">
-        <v>130</v>
+        <v>42</v>
       </c>
       <c r="D3" s="40"/>
       <c r="E3" s="40"/>
@@ -2573,7 +2567,7 @@
       <c r="J3" s="40"/>
       <c r="K3" s="40"/>
       <c r="L3" s="41" t="s">
-        <v>131</v>
+        <v>43</v>
       </c>
       <c r="M3" s="42"/>
       <c r="N3" s="42"/>
@@ -2586,816 +2580,816 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>44</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>133</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>134</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>135</v>
+        <v>47</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>133</v>
+        <v>45</v>
       </c>
       <c r="G4" t="s">
-        <v>134</v>
+        <v>46</v>
       </c>
       <c r="H4" t="s">
-        <v>135</v>
+        <v>47</v>
       </c>
       <c r="I4" s="25" t="s">
-        <v>133</v>
+        <v>45</v>
       </c>
       <c r="J4" t="s">
-        <v>134</v>
+        <v>46</v>
       </c>
       <c r="K4" t="s">
-        <v>135</v>
+        <v>47</v>
       </c>
       <c r="L4" s="25" t="s">
-        <v>133</v>
+        <v>45</v>
       </c>
       <c r="M4" t="s">
-        <v>134</v>
+        <v>46</v>
       </c>
       <c r="N4" t="s">
-        <v>135</v>
+        <v>47</v>
       </c>
       <c r="O4" s="25" t="s">
-        <v>133</v>
+        <v>45</v>
       </c>
       <c r="P4" t="s">
-        <v>134</v>
+        <v>46</v>
       </c>
       <c r="Q4" t="s">
-        <v>135</v>
+        <v>47</v>
       </c>
       <c r="R4" s="25" t="s">
-        <v>133</v>
+        <v>45</v>
       </c>
       <c r="S4" t="s">
-        <v>134</v>
+        <v>46</v>
       </c>
       <c r="T4" t="s">
-        <v>135</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>138</v>
+        <v>49</v>
+      </c>
+      <c r="C5" s="25">
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>140</v>
-      </c>
-      <c r="F5" s="25" t="s">
-        <v>141</v>
+        <v>51</v>
+      </c>
+      <c r="F5" s="25">
+        <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>142</v>
+        <v>52</v>
       </c>
       <c r="H5" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="I5" s="25">
         <v>4</v>
       </c>
       <c r="J5" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="K5" t="s">
-        <v>145</v>
-      </c>
-      <c r="L5" s="25" t="s">
-        <v>138</v>
+        <v>55</v>
+      </c>
+      <c r="L5" s="25">
+        <v>2</v>
       </c>
       <c r="M5" t="s">
-        <v>146</v>
+        <v>56</v>
       </c>
       <c r="N5" t="s">
-        <v>147</v>
-      </c>
-      <c r="O5" s="25" t="s">
-        <v>141</v>
+        <v>57</v>
+      </c>
+      <c r="O5" s="25">
+        <v>3</v>
       </c>
       <c r="P5" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
       <c r="Q5" t="s">
-        <v>149</v>
+        <v>59</v>
       </c>
       <c r="R5" s="25">
         <v>4</v>
       </c>
       <c r="S5" t="s">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="T5" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>153</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>138</v>
+        <v>63</v>
+      </c>
+      <c r="C6" s="25">
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>145</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>141</v>
+        <v>55</v>
+      </c>
+      <c r="F6" s="25">
+        <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="H6" t="s">
-        <v>146</v>
+        <v>56</v>
       </c>
       <c r="I6" s="25">
         <v>4</v>
       </c>
       <c r="J6" t="s">
-        <v>149</v>
+        <v>59</v>
       </c>
       <c r="K6" t="s">
-        <v>140</v>
-      </c>
-      <c r="L6" s="25" t="s">
-        <v>138</v>
+        <v>51</v>
+      </c>
+      <c r="L6" s="25">
+        <v>2</v>
       </c>
       <c r="M6" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
       <c r="N6" t="s">
-        <v>144</v>
-      </c>
-      <c r="O6" s="25" t="s">
-        <v>141</v>
+        <v>54</v>
+      </c>
+      <c r="O6" s="25">
+        <v>3</v>
       </c>
       <c r="P6" t="s">
-        <v>147</v>
+        <v>57</v>
       </c>
       <c r="Q6" t="s">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="R6" s="25">
         <v>4</v>
       </c>
       <c r="S6" t="s">
-        <v>142</v>
+        <v>52</v>
       </c>
       <c r="T6" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>154</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>138</v>
+        <v>49</v>
+      </c>
+      <c r="C7" s="25">
+        <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>149</v>
-      </c>
-      <c r="F7" s="25" t="s">
-        <v>141</v>
+        <v>59</v>
+      </c>
+      <c r="F7" s="25">
+        <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>146</v>
+        <v>56</v>
       </c>
       <c r="H7" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="I7" s="25">
         <v>4</v>
       </c>
       <c r="J7" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="K7" t="s">
-        <v>148</v>
-      </c>
-      <c r="L7" s="25" t="s">
-        <v>138</v>
+        <v>58</v>
+      </c>
+      <c r="L7" s="25">
+        <v>2</v>
       </c>
       <c r="M7" t="s">
-        <v>142</v>
+        <v>52</v>
       </c>
       <c r="N7" t="s">
-        <v>140</v>
-      </c>
-      <c r="O7" s="25" t="s">
-        <v>141</v>
+        <v>51</v>
+      </c>
+      <c r="O7" s="25">
+        <v>3</v>
       </c>
       <c r="P7" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="Q7" t="s">
-        <v>147</v>
+        <v>57</v>
       </c>
       <c r="R7" s="25">
         <v>4</v>
       </c>
       <c r="S7" t="s">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="T7" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>153</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>138</v>
+        <v>63</v>
+      </c>
+      <c r="C8" s="25">
+        <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>147</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>148</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>141</v>
+        <v>58</v>
+      </c>
+      <c r="F8" s="25">
+        <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
       <c r="H8" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="I8" s="25">
         <v>4</v>
       </c>
       <c r="J8" t="s">
-        <v>146</v>
+        <v>56</v>
       </c>
       <c r="K8" t="s">
-        <v>142</v>
-      </c>
-      <c r="L8" s="25" t="s">
-        <v>138</v>
+        <v>52</v>
+      </c>
+      <c r="L8" s="25">
+        <v>2</v>
       </c>
       <c r="M8" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="N8" t="s">
-        <v>150</v>
-      </c>
-      <c r="O8" s="25" t="s">
-        <v>141</v>
+        <v>60</v>
+      </c>
+      <c r="O8" s="25">
+        <v>3</v>
       </c>
       <c r="P8" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="Q8" t="s">
-        <v>149</v>
+        <v>59</v>
       </c>
       <c r="R8" s="25">
         <v>4</v>
       </c>
       <c r="S8" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="T8" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>156</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>137</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>138</v>
+        <v>49</v>
+      </c>
+      <c r="C9" s="25">
+        <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="E9" t="s">
-        <v>142</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>141</v>
+        <v>52</v>
+      </c>
+      <c r="F9" s="25">
+        <v>3</v>
       </c>
       <c r="G9" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="H9" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="I9" s="25">
         <v>4</v>
       </c>
       <c r="J9" t="s">
-        <v>147</v>
+        <v>57</v>
       </c>
       <c r="K9" t="s">
-        <v>149</v>
-      </c>
-      <c r="L9" s="25" t="s">
-        <v>138</v>
+        <v>59</v>
+      </c>
+      <c r="L9" s="25">
+        <v>2</v>
       </c>
       <c r="M9" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
       <c r="N9" t="s">
-        <v>143</v>
-      </c>
-      <c r="O9" s="25" t="s">
-        <v>141</v>
+        <v>53</v>
+      </c>
+      <c r="O9" s="25">
+        <v>3</v>
       </c>
       <c r="P9" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="Q9" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="R9" s="25">
         <v>4</v>
       </c>
       <c r="S9" t="s">
-        <v>146</v>
+        <v>56</v>
       </c>
       <c r="T9" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>157</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>138</v>
+        <v>63</v>
+      </c>
+      <c r="C10" s="25">
+        <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>146</v>
-      </c>
-      <c r="F10" s="25" t="s">
-        <v>141</v>
+        <v>56</v>
+      </c>
+      <c r="F10" s="25">
+        <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
       <c r="H10" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="I10" s="25">
         <v>4</v>
       </c>
       <c r="J10" t="s">
-        <v>147</v>
+        <v>57</v>
       </c>
       <c r="K10" t="s">
-        <v>144</v>
-      </c>
-      <c r="L10" s="25" t="s">
-        <v>138</v>
+        <v>54</v>
+      </c>
+      <c r="L10" s="25">
+        <v>2</v>
       </c>
       <c r="M10" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="N10" t="s">
-        <v>142</v>
-      </c>
-      <c r="O10" s="25" t="s">
-        <v>141</v>
+        <v>52</v>
+      </c>
+      <c r="O10" s="25">
+        <v>3</v>
       </c>
       <c r="P10" t="s">
-        <v>149</v>
+        <v>59</v>
       </c>
       <c r="Q10" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="R10" s="25">
         <v>4</v>
       </c>
       <c r="S10" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="T10" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>158</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>138</v>
+        <v>49</v>
+      </c>
+      <c r="C11" s="25">
+        <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>144</v>
-      </c>
-      <c r="F11" s="25" t="s">
-        <v>141</v>
+        <v>54</v>
+      </c>
+      <c r="F11" s="25">
+        <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="H11" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
       <c r="I11" s="25">
         <v>4</v>
       </c>
       <c r="J11" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
       <c r="K11" t="s">
-        <v>142</v>
-      </c>
-      <c r="L11" s="25" t="s">
-        <v>138</v>
+        <v>52</v>
+      </c>
+      <c r="L11" s="25">
+        <v>2</v>
       </c>
       <c r="M11" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="N11" t="s">
-        <v>146</v>
-      </c>
-      <c r="O11" s="25" t="s">
-        <v>141</v>
+        <v>56</v>
+      </c>
+      <c r="O11" s="25">
+        <v>3</v>
       </c>
       <c r="P11" t="s">
-        <v>149</v>
+        <v>59</v>
       </c>
       <c r="Q11" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="R11" s="25">
         <v>4</v>
       </c>
       <c r="S11" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="T11" t="s">
-        <v>147</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>159</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>153</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>138</v>
+        <v>63</v>
+      </c>
+      <c r="C12" s="25">
+        <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="E12" t="s">
-        <v>151</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>141</v>
+        <v>61</v>
+      </c>
+      <c r="F12" s="25">
+        <v>3</v>
       </c>
       <c r="G12" t="s">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="H12" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="I12" s="25">
         <v>4</v>
       </c>
       <c r="J12" t="s">
-        <v>142</v>
+        <v>52</v>
       </c>
       <c r="K12" t="s">
-        <v>149</v>
-      </c>
-      <c r="L12" s="25" t="s">
-        <v>138</v>
+        <v>59</v>
+      </c>
+      <c r="L12" s="25">
+        <v>2</v>
       </c>
       <c r="M12" t="s">
-        <v>147</v>
+        <v>57</v>
       </c>
       <c r="N12" t="s">
-        <v>140</v>
-      </c>
-      <c r="O12" s="25" t="s">
-        <v>141</v>
+        <v>51</v>
+      </c>
+      <c r="O12" s="25">
+        <v>3</v>
       </c>
       <c r="P12" t="s">
-        <v>146</v>
+        <v>56</v>
       </c>
       <c r="Q12" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
       <c r="R12" s="25">
         <v>4</v>
       </c>
       <c r="S12" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="T12" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>160</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>138</v>
+        <v>49</v>
+      </c>
+      <c r="C13" s="25">
+        <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>151</v>
-      </c>
-      <c r="F13" s="25" t="s">
-        <v>141</v>
+        <v>61</v>
+      </c>
+      <c r="F13" s="25">
+        <v>3</v>
       </c>
       <c r="G13" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="H13" t="s">
-        <v>147</v>
+        <v>57</v>
       </c>
       <c r="I13" s="25">
         <v>4</v>
       </c>
       <c r="J13" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
       <c r="K13" t="s">
-        <v>150</v>
-      </c>
-      <c r="L13" s="25" t="s">
-        <v>138</v>
+        <v>60</v>
+      </c>
+      <c r="L13" s="25">
+        <v>2</v>
       </c>
       <c r="M13" t="s">
-        <v>149</v>
+        <v>59</v>
       </c>
       <c r="N13" t="s">
-        <v>146</v>
-      </c>
-      <c r="O13" s="25" t="s">
-        <v>141</v>
+        <v>56</v>
+      </c>
+      <c r="O13" s="25">
+        <v>3</v>
       </c>
       <c r="P13" t="s">
-        <v>142</v>
+        <v>52</v>
       </c>
       <c r="Q13" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="R13" s="25">
         <v>4</v>
       </c>
       <c r="S13" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
       <c r="T13" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>161</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>153</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>138</v>
+        <v>63</v>
+      </c>
+      <c r="C14" s="25">
+        <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F14" s="25" t="s">
-        <v>141</v>
+        <v>57</v>
+      </c>
+      <c r="F14" s="25">
+        <v>3</v>
       </c>
       <c r="G14" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
       <c r="H14" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="I14" s="25">
         <v>4</v>
       </c>
       <c r="J14" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="K14" t="s">
-        <v>146</v>
-      </c>
-      <c r="L14" s="25" t="s">
-        <v>138</v>
+        <v>56</v>
+      </c>
+      <c r="L14" s="25">
+        <v>2</v>
       </c>
       <c r="M14" t="s">
-        <v>149</v>
+        <v>59</v>
       </c>
       <c r="N14" t="s">
-        <v>150</v>
-      </c>
-      <c r="O14" s="25" t="s">
-        <v>141</v>
+        <v>60</v>
+      </c>
+      <c r="O14" s="25">
+        <v>3</v>
       </c>
       <c r="P14" t="s">
-        <v>142</v>
+        <v>52</v>
       </c>
       <c r="Q14" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="R14" s="25">
         <v>4</v>
       </c>
       <c r="S14" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="T14" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>138</v>
+        <v>49</v>
+      </c>
+      <c r="C15" s="25">
+        <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>140</v>
-      </c>
-      <c r="F15" s="25" t="s">
-        <v>141</v>
+        <v>51</v>
+      </c>
+      <c r="F15" s="25">
+        <v>3</v>
       </c>
       <c r="G15" t="s">
-        <v>149</v>
+        <v>59</v>
       </c>
       <c r="H15" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="I15" s="25">
         <v>4</v>
       </c>
       <c r="J15" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="K15" t="s">
-        <v>143</v>
-      </c>
-      <c r="L15" s="25" t="s">
-        <v>138</v>
+        <v>53</v>
+      </c>
+      <c r="L15" s="25">
+        <v>2</v>
       </c>
       <c r="M15" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="N15" t="s">
-        <v>150</v>
-      </c>
-      <c r="O15" s="25" t="s">
-        <v>141</v>
+        <v>60</v>
+      </c>
+      <c r="O15" s="25">
+        <v>3</v>
       </c>
       <c r="P15" t="s">
-        <v>142</v>
+        <v>52</v>
       </c>
       <c r="Q15" t="s">
-        <v>147</v>
+        <v>57</v>
       </c>
       <c r="R15" s="25">
         <v>4</v>
       </c>
       <c r="S15" t="s">
-        <v>146</v>
+        <v>56</v>
       </c>
       <c r="T15" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>163</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>153</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>138</v>
+        <v>63</v>
+      </c>
+      <c r="C16" s="25">
+        <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>149</v>
+        <v>59</v>
       </c>
       <c r="E16" t="s">
-        <v>148</v>
-      </c>
-      <c r="F16" s="25" t="s">
-        <v>141</v>
+        <v>58</v>
+      </c>
+      <c r="F16" s="25">
+        <v>3</v>
       </c>
       <c r="G16" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="H16" t="s">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="I16" s="25">
         <v>4</v>
       </c>
       <c r="J16" t="s">
-        <v>147</v>
+        <v>57</v>
       </c>
       <c r="K16" t="s">
-        <v>146</v>
-      </c>
-      <c r="L16" s="25" t="s">
-        <v>138</v>
+        <v>56</v>
+      </c>
+      <c r="L16" s="25">
+        <v>2</v>
       </c>
       <c r="M16" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="N16" t="s">
-        <v>142</v>
-      </c>
-      <c r="O16" s="25" t="s">
-        <v>141</v>
+        <v>52</v>
+      </c>
+      <c r="O16" s="25">
+        <v>3</v>
       </c>
       <c r="P16" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
       <c r="Q16" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="R16" s="25">
         <v>4</v>
       </c>
       <c r="S16" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="T16" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>164</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>49</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>165</v>
+        <v>75</v>
       </c>
       <c r="D17" s="36"/>
       <c r="E17" s="36"/>
@@ -3417,633 +3411,633 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>153</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>138</v>
+        <v>63</v>
+      </c>
+      <c r="C18" s="25">
+        <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>142</v>
-      </c>
-      <c r="F18" s="25" t="s">
-        <v>141</v>
+        <v>52</v>
+      </c>
+      <c r="F18" s="25">
+        <v>3</v>
       </c>
       <c r="G18" t="s">
-        <v>146</v>
+        <v>56</v>
       </c>
       <c r="H18" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="I18" s="25">
         <v>4</v>
       </c>
       <c r="J18" t="s">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="K18" t="s">
-        <v>147</v>
-      </c>
-      <c r="L18" s="25" t="s">
-        <v>138</v>
+        <v>57</v>
+      </c>
+      <c r="L18" s="25">
+        <v>2</v>
       </c>
       <c r="M18" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="N18" t="s">
-        <v>151</v>
-      </c>
-      <c r="O18" s="25" t="s">
-        <v>141</v>
+        <v>61</v>
+      </c>
+      <c r="O18" s="25">
+        <v>3</v>
       </c>
       <c r="P18" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="Q18" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
       <c r="R18" s="25">
         <v>4</v>
       </c>
       <c r="S18" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
       <c r="T18" t="s">
-        <v>149</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>167</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>137</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>138</v>
+        <v>49</v>
+      </c>
+      <c r="C19" s="25">
+        <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>147</v>
+        <v>57</v>
       </c>
       <c r="E19" t="s">
-        <v>145</v>
-      </c>
-      <c r="F19" s="25" t="s">
-        <v>141</v>
+        <v>55</v>
+      </c>
+      <c r="F19" s="25">
+        <v>3</v>
       </c>
       <c r="G19" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
       <c r="H19" t="s">
-        <v>142</v>
+        <v>52</v>
       </c>
       <c r="I19" s="25">
         <v>4</v>
       </c>
       <c r="J19" t="s">
-        <v>149</v>
+        <v>59</v>
       </c>
       <c r="K19" t="s">
-        <v>144</v>
-      </c>
-      <c r="L19" s="25" t="s">
-        <v>138</v>
+        <v>54</v>
+      </c>
+      <c r="L19" s="25">
+        <v>2</v>
       </c>
       <c r="M19" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="N19" t="s">
-        <v>150</v>
-      </c>
-      <c r="O19" s="25" t="s">
-        <v>141</v>
+        <v>60</v>
+      </c>
+      <c r="O19" s="25">
+        <v>3</v>
       </c>
       <c r="P19" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="Q19" t="s">
-        <v>146</v>
+        <v>56</v>
       </c>
       <c r="R19" s="25">
         <v>4</v>
       </c>
       <c r="S19" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
       <c r="T19" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>168</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>153</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>138</v>
+        <v>63</v>
+      </c>
+      <c r="C20" s="25">
+        <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>140</v>
-      </c>
-      <c r="F20" s="25" t="s">
-        <v>141</v>
+        <v>51</v>
+      </c>
+      <c r="F20" s="25">
+        <v>3</v>
       </c>
       <c r="G20" t="s">
-        <v>149</v>
+        <v>59</v>
       </c>
       <c r="H20" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="I20" s="25">
         <v>4</v>
       </c>
       <c r="J20" t="s">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="K20" t="s">
-        <v>139</v>
-      </c>
-      <c r="L20" s="25" t="s">
-        <v>138</v>
+        <v>50</v>
+      </c>
+      <c r="L20" s="25">
+        <v>2</v>
       </c>
       <c r="M20" t="s">
-        <v>142</v>
+        <v>52</v>
       </c>
       <c r="N20" t="s">
-        <v>146</v>
-      </c>
-      <c r="O20" s="25" t="s">
-        <v>141</v>
+        <v>56</v>
+      </c>
+      <c r="O20" s="25">
+        <v>3</v>
       </c>
       <c r="P20" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
       <c r="Q20" t="s">
-        <v>147</v>
+        <v>57</v>
       </c>
       <c r="R20" s="25">
         <v>4</v>
       </c>
       <c r="S20" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="T20" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>169</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
-        <v>137</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>138</v>
+        <v>49</v>
+      </c>
+      <c r="C21" s="25">
+        <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="E21" t="s">
-        <v>144</v>
-      </c>
-      <c r="F21" s="25" t="s">
-        <v>141</v>
+        <v>54</v>
+      </c>
+      <c r="F21" s="25">
+        <v>3</v>
       </c>
       <c r="G21" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="H21" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
       <c r="I21" s="25">
         <v>4</v>
       </c>
       <c r="J21" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
       <c r="K21" t="s">
-        <v>146</v>
-      </c>
-      <c r="L21" s="25" t="s">
-        <v>138</v>
+        <v>56</v>
+      </c>
+      <c r="L21" s="25">
+        <v>2</v>
       </c>
       <c r="M21" t="s">
-        <v>149</v>
+        <v>59</v>
       </c>
       <c r="N21" t="s">
-        <v>147</v>
-      </c>
-      <c r="O21" s="25" t="s">
-        <v>141</v>
+        <v>57</v>
+      </c>
+      <c r="O21" s="25">
+        <v>3</v>
       </c>
       <c r="P21" t="s">
-        <v>142</v>
+        <v>52</v>
       </c>
       <c r="Q21" t="s">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="R21" s="25">
         <v>4</v>
       </c>
       <c r="S21" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="T21" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>153</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>138</v>
+        <v>63</v>
+      </c>
+      <c r="C22" s="25">
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>149</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>141</v>
+        <v>59</v>
+      </c>
+      <c r="F22" s="25">
+        <v>3</v>
       </c>
       <c r="G22" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
       <c r="H22" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="I22" s="25">
         <v>4</v>
       </c>
       <c r="J22" t="s">
-        <v>142</v>
+        <v>52</v>
       </c>
       <c r="K22" t="s">
-        <v>145</v>
-      </c>
-      <c r="L22" s="25" t="s">
-        <v>138</v>
+        <v>55</v>
+      </c>
+      <c r="L22" s="25">
+        <v>2</v>
       </c>
       <c r="M22" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="N22" t="s">
-        <v>140</v>
-      </c>
-      <c r="O22" s="25" t="s">
-        <v>141</v>
+        <v>51</v>
+      </c>
+      <c r="O22" s="25">
+        <v>3</v>
       </c>
       <c r="P22" t="s">
-        <v>146</v>
+        <v>56</v>
       </c>
       <c r="Q22" t="s">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="R22" s="25">
         <v>4</v>
       </c>
       <c r="S22" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="T22" t="s">
-        <v>147</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>171</v>
+        <v>81</v>
       </c>
       <c r="B23" t="s">
-        <v>137</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>138</v>
+        <v>49</v>
+      </c>
+      <c r="C23" s="25">
+        <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>146</v>
+        <v>56</v>
       </c>
       <c r="E23" t="s">
-        <v>145</v>
-      </c>
-      <c r="F23" s="25" t="s">
-        <v>141</v>
+        <v>55</v>
+      </c>
+      <c r="F23" s="25">
+        <v>3</v>
       </c>
       <c r="G23" t="s">
-        <v>147</v>
+        <v>57</v>
       </c>
       <c r="H23" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="I23" s="25">
         <v>4</v>
       </c>
       <c r="J23" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
       <c r="K23" t="s">
-        <v>150</v>
-      </c>
-      <c r="L23" s="25" t="s">
-        <v>138</v>
+        <v>60</v>
+      </c>
+      <c r="L23" s="25">
+        <v>2</v>
       </c>
       <c r="M23" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="N23" t="s">
-        <v>149</v>
-      </c>
-      <c r="O23" s="25" t="s">
-        <v>141</v>
+        <v>59</v>
+      </c>
+      <c r="O23" s="25">
+        <v>3</v>
       </c>
       <c r="P23" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="Q23" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="R23" s="25">
         <v>4</v>
       </c>
       <c r="S23" t="s">
-        <v>142</v>
+        <v>52</v>
       </c>
       <c r="T23" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>172</v>
+        <v>82</v>
       </c>
       <c r="B24" t="s">
-        <v>153</v>
-      </c>
-      <c r="C24" s="25" t="s">
-        <v>138</v>
+        <v>63</v>
+      </c>
+      <c r="C24" s="25">
+        <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
       <c r="E24" t="s">
-        <v>146</v>
-      </c>
-      <c r="F24" s="25" t="s">
-        <v>141</v>
+        <v>56</v>
+      </c>
+      <c r="F24" s="25">
+        <v>3</v>
       </c>
       <c r="G24" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="H24" t="s">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="I24" s="25">
         <v>4</v>
       </c>
       <c r="J24" t="s">
-        <v>149</v>
+        <v>59</v>
       </c>
       <c r="K24" t="s">
-        <v>142</v>
-      </c>
-      <c r="L24" s="25" t="s">
-        <v>138</v>
+        <v>52</v>
+      </c>
+      <c r="L24" s="25">
+        <v>2</v>
       </c>
       <c r="M24" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="N24" t="s">
-        <v>139</v>
-      </c>
-      <c r="O24" s="25" t="s">
-        <v>141</v>
+        <v>50</v>
+      </c>
+      <c r="O24" s="25">
+        <v>3</v>
       </c>
       <c r="P24" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
       <c r="Q24" t="s">
-        <v>147</v>
+        <v>57</v>
       </c>
       <c r="R24" s="25">
         <v>4</v>
       </c>
       <c r="S24" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="T24" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>173</v>
+        <v>83</v>
       </c>
       <c r="B25" t="s">
-        <v>137</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>138</v>
+        <v>49</v>
+      </c>
+      <c r="C25" s="25">
+        <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>147</v>
+        <v>57</v>
       </c>
       <c r="E25" t="s">
-        <v>143</v>
-      </c>
-      <c r="F25" s="25" t="s">
-        <v>141</v>
+        <v>53</v>
+      </c>
+      <c r="F25" s="25">
+        <v>3</v>
       </c>
       <c r="G25" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="H25" t="s">
-        <v>142</v>
+        <v>52</v>
       </c>
       <c r="I25" s="25">
         <v>4</v>
       </c>
       <c r="J25" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="K25" t="s">
-        <v>139</v>
-      </c>
-      <c r="L25" s="25" t="s">
-        <v>138</v>
+        <v>50</v>
+      </c>
+      <c r="L25" s="25">
+        <v>2</v>
       </c>
       <c r="M25" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="N25" t="s">
-        <v>140</v>
-      </c>
-      <c r="O25" s="25" t="s">
-        <v>141</v>
+        <v>51</v>
+      </c>
+      <c r="O25" s="25">
+        <v>3</v>
       </c>
       <c r="P25" t="s">
-        <v>146</v>
+        <v>56</v>
       </c>
       <c r="Q25" t="s">
-        <v>149</v>
+        <v>59</v>
       </c>
       <c r="R25" s="25">
         <v>4</v>
       </c>
       <c r="S25" t="s">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="T25" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>174</v>
+        <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>153</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>138</v>
+        <v>63</v>
+      </c>
+      <c r="C26" s="25">
+        <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="E26" t="s">
-        <v>148</v>
-      </c>
-      <c r="F26" s="25" t="s">
-        <v>141</v>
+        <v>58</v>
+      </c>
+      <c r="F26" s="25">
+        <v>3</v>
       </c>
       <c r="G26" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
       <c r="H26" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="I26" s="25">
         <v>4</v>
       </c>
       <c r="J26" t="s">
-        <v>147</v>
+        <v>57</v>
       </c>
       <c r="K26" t="s">
-        <v>139</v>
-      </c>
-      <c r="L26" s="25" t="s">
-        <v>138</v>
+        <v>50</v>
+      </c>
+      <c r="L26" s="25">
+        <v>2</v>
       </c>
       <c r="M26" t="s">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="N26" t="s">
-        <v>149</v>
-      </c>
-      <c r="O26" s="25" t="s">
-        <v>141</v>
+        <v>59</v>
+      </c>
+      <c r="O26" s="25">
+        <v>3</v>
       </c>
       <c r="P26" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="Q26" t="s">
-        <v>142</v>
+        <v>52</v>
       </c>
       <c r="R26" s="25">
         <v>4</v>
       </c>
       <c r="S26" t="s">
-        <v>146</v>
+        <v>56</v>
       </c>
       <c r="T26" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>175</v>
+        <v>85</v>
       </c>
       <c r="B27" t="s">
-        <v>137</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>138</v>
+        <v>49</v>
+      </c>
+      <c r="C27" s="25">
+        <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>147</v>
+        <v>57</v>
       </c>
       <c r="E27" t="s">
-        <v>142</v>
-      </c>
-      <c r="F27" s="25" t="s">
-        <v>141</v>
+        <v>52</v>
+      </c>
+      <c r="F27" s="25">
+        <v>3</v>
       </c>
       <c r="G27" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="H27" t="s">
-        <v>149</v>
+        <v>59</v>
       </c>
       <c r="I27" s="25">
         <v>4</v>
       </c>
       <c r="J27" t="s">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="K27" t="s">
-        <v>144</v>
-      </c>
-      <c r="L27" s="25" t="s">
-        <v>138</v>
+        <v>54</v>
+      </c>
+      <c r="L27" s="25">
+        <v>2</v>
       </c>
       <c r="M27" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
       <c r="N27" t="s">
-        <v>148</v>
-      </c>
-      <c r="O27" s="25" t="s">
-        <v>141</v>
+        <v>58</v>
+      </c>
+      <c r="O27" s="25">
+        <v>3</v>
       </c>
       <c r="P27" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="Q27" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="R27" s="25">
         <v>4</v>
       </c>
       <c r="S27" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="T27" t="s">
-        <v>146</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
-        <v>176</v>
+        <v>86</v>
       </c>
       <c r="B28" t="s">
-        <v>137</v>
+        <v>49</v>
       </c>
       <c r="C28" s="35" t="s">
-        <v>117</v>
+        <v>29</v>
       </c>
       <c r="D28" s="36"/>
       <c r="E28" s="36"/>
@@ -4065,13 +4059,13 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
-        <v>177</v>
+        <v>87</v>
       </c>
       <c r="B29" t="s">
-        <v>137</v>
+        <v>49</v>
       </c>
       <c r="C29" s="35" t="s">
-        <v>118</v>
+        <v>30</v>
       </c>
       <c r="D29" s="36"/>
       <c r="E29" s="36"/>
@@ -4093,13 +4087,13 @@
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
-        <v>178</v>
+        <v>88</v>
       </c>
       <c r="B30" t="s">
-        <v>137</v>
+        <v>49</v>
       </c>
       <c r="C30" s="35" t="s">
-        <v>121</v>
+        <v>33</v>
       </c>
       <c r="D30" s="36"/>
       <c r="E30" s="36"/>
@@ -4121,13 +4115,13 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
-        <v>179</v>
+        <v>89</v>
       </c>
       <c r="B31" t="s">
-        <v>137</v>
+        <v>49</v>
       </c>
       <c r="C31" s="35" t="s">
-        <v>121</v>
+        <v>33</v>
       </c>
       <c r="D31" s="36"/>
       <c r="E31" s="36"/>
@@ -4149,13 +4143,13 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="B32" t="s">
-        <v>137</v>
+        <v>49</v>
       </c>
       <c r="C32" s="35" t="s">
-        <v>124</v>
+        <v>36</v>
       </c>
       <c r="D32" s="36"/>
       <c r="E32" s="36"/>
@@ -4177,13 +4171,13 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
-        <v>181</v>
+        <v>91</v>
       </c>
       <c r="B33" t="s">
-        <v>137</v>
+        <v>49</v>
       </c>
       <c r="C33" s="35" t="s">
-        <v>124</v>
+        <v>36</v>
       </c>
       <c r="D33" s="36"/>
       <c r="E33" s="36"/>
@@ -4205,17 +4199,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C29:S29"/>
+    <mergeCell ref="C30:S30"/>
+    <mergeCell ref="C31:S31"/>
+    <mergeCell ref="C32:S32"/>
+    <mergeCell ref="C33:S33"/>
     <mergeCell ref="C28:S28"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="C3:K3"/>
     <mergeCell ref="L3:T3"/>
     <mergeCell ref="C17:S17"/>
-    <mergeCell ref="C29:S29"/>
-    <mergeCell ref="C30:S30"/>
-    <mergeCell ref="C31:S31"/>
-    <mergeCell ref="C32:S32"/>
-    <mergeCell ref="C33:S33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>